<commit_message>
xls 2007 test file
</commit_message>
<xml_diff>
--- a/data-converters/src/test/resources/xls/simple.xlsx
+++ b/data-converters/src/test/resources/xls/simple.xlsx
@@ -4,19 +4,17 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="15195" windowHeight="6405"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9375" windowHeight="5265"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="simple" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>Nazwa</t>
   </si>
@@ -39,78 +37,228 @@
     <t>Kryterium6</t>
   </si>
   <si>
+    <t>Alternatywa 1</t>
+  </si>
+  <si>
+    <t>Alternatywa 2</t>
+  </si>
+  <si>
+    <t>Alternatywa 3</t>
+  </si>
+  <si>
+    <t>Alternatywa 4</t>
+  </si>
+  <si>
+    <t>Alternatywa 5</t>
+  </si>
+  <si>
+    <t>Alternatywa 6</t>
+  </si>
+  <si>
+    <t>Alternatywa 7</t>
+  </si>
+  <si>
+    <t>Alternatywa 8</t>
+  </si>
+  <si>
+    <t>Alternatywa 9</t>
+  </si>
+  <si>
+    <t>Wartosc A11</t>
+  </si>
+  <si>
+    <t>Wartosc A21</t>
+  </si>
+  <si>
+    <t>Wartosc A31</t>
+  </si>
+  <si>
+    <t>Wartosc A41</t>
+  </si>
+  <si>
+    <t>Wartosc A51</t>
+  </si>
+  <si>
+    <t>Wartosc A61</t>
+  </si>
+  <si>
+    <t>Wartosc A71</t>
+  </si>
+  <si>
+    <t>Wartosc A81</t>
+  </si>
+  <si>
+    <t>Wartosc A91</t>
+  </si>
+  <si>
+    <t>Wartosc A12</t>
+  </si>
+  <si>
+    <t>Wartosc A13</t>
+  </si>
+  <si>
+    <t>Wartosc A14</t>
+  </si>
+  <si>
+    <t>Wartosc A15</t>
+  </si>
+  <si>
+    <t>Wartosc A16</t>
+  </si>
+  <si>
+    <t>Wartosc A22</t>
+  </si>
+  <si>
+    <t>Wartosc A23</t>
+  </si>
+  <si>
+    <t>Wartosc A24</t>
+  </si>
+  <si>
+    <t>Wartosc A25</t>
+  </si>
+  <si>
+    <t>Wartosc A26</t>
+  </si>
+  <si>
+    <t>Wartosc A32</t>
+  </si>
+  <si>
+    <t>Wartosc A33</t>
+  </si>
+  <si>
+    <t>Wartosc A34</t>
+  </si>
+  <si>
+    <t>Wartosc A35</t>
+  </si>
+  <si>
+    <t>Wartosc A36</t>
+  </si>
+  <si>
+    <t>Wartosc A42</t>
+  </si>
+  <si>
+    <t>Wartosc A43</t>
+  </si>
+  <si>
+    <t>Wartosc A44</t>
+  </si>
+  <si>
+    <t>Wartosc A45</t>
+  </si>
+  <si>
+    <t>Wartosc A46</t>
+  </si>
+  <si>
+    <t>Wartosc A52</t>
+  </si>
+  <si>
+    <t>Wartosc A53</t>
+  </si>
+  <si>
+    <t>Wartosc A54</t>
+  </si>
+  <si>
+    <t>Wartosc A55</t>
+  </si>
+  <si>
+    <t>Wartosc A56</t>
+  </si>
+  <si>
+    <t>Wartosc A62</t>
+  </si>
+  <si>
+    <t>Wartosc A63</t>
+  </si>
+  <si>
+    <t>Wartosc A64</t>
+  </si>
+  <si>
+    <t>Wartosc A65</t>
+  </si>
+  <si>
+    <t>Wartosc A66</t>
+  </si>
+  <si>
+    <t>Wartosc A72</t>
+  </si>
+  <si>
+    <t>Wartosc A73</t>
+  </si>
+  <si>
+    <t>Wartosc A74</t>
+  </si>
+  <si>
+    <t>Wartosc A75</t>
+  </si>
+  <si>
+    <t>Wartosc A76</t>
+  </si>
+  <si>
+    <t>Wartosc A82</t>
+  </si>
+  <si>
+    <t>Wartosc A83</t>
+  </si>
+  <si>
+    <t>Wartosc A84</t>
+  </si>
+  <si>
+    <t>Wartosc A85</t>
+  </si>
+  <si>
+    <t>Wartosc A86</t>
+  </si>
+  <si>
+    <t>Wartosc A92</t>
+  </si>
+  <si>
+    <t>Wartosc A93</t>
+  </si>
+  <si>
+    <t>Wartosc A94</t>
+  </si>
+  <si>
+    <t>Wartosc A95</t>
+  </si>
+  <si>
+    <t>Wartosc A96</t>
+  </si>
+  <si>
     <t>g</t>
   </si>
   <si>
-    <t>c,2</t>
-  </si>
-  <si>
-    <t>g ,  3</t>
-  </si>
-  <si>
-    <t>c   .    4</t>
-  </si>
-  <si>
     <t>c</t>
   </si>
   <si>
     <t>g,1</t>
   </si>
   <si>
-    <t>Alternatywa1</t>
-  </si>
-  <si>
-    <t>Alternatywa2</t>
-  </si>
-  <si>
-    <t>Wartosc11</t>
-  </si>
-  <si>
-    <t>Wartosc12</t>
-  </si>
-  <si>
-    <t>Wartosc13</t>
-  </si>
-  <si>
-    <t>Wartosc14</t>
-  </si>
-  <si>
-    <t>Wartosc15</t>
-  </si>
-  <si>
-    <t>Wartosc16</t>
-  </si>
-  <si>
-    <t>Wartosc21</t>
-  </si>
-  <si>
-    <t>Wartosc22</t>
-  </si>
-  <si>
-    <t>Wartosc23</t>
-  </si>
-  <si>
-    <t>Wartosc24</t>
-  </si>
-  <si>
-    <t>Wartosc25</t>
-  </si>
-  <si>
-    <t>Wartosc26</t>
+    <t>c , 2</t>
+  </si>
+  <si>
+    <t>g  ,  3</t>
+  </si>
+  <si>
+    <t>c    ,    4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <charset val="238"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,8 +281,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,84 +578,114 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H5"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="2" max="8" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:8">
+      <c r="C1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H1" t="s">
+        <v>75</v>
+      </c>
+    </row>
     <row r="2" spans="1:8">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
       <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="E4" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="F4" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="H4" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -514,52 +693,175 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" t="s">
+        <v>51</v>
+      </c>
+      <c r="F8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="B10" t="s">
         <v>14</v>
       </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="F5" t="s">
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" t="s">
+        <v>63</v>
+      </c>
+      <c r="H10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s">
         <v>24</v>
       </c>
-      <c r="G5" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" t="s">
-        <v>26</v>
+      <c r="D11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E11" t="s">
+        <v>66</v>
+      </c>
+      <c r="F11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="0" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>